<commit_message>
update insert_client function to include idx parameter and adjust related notebook cells
</commit_message>
<xml_diff>
--- a/src/inserted/contrato_insert_sucess.xlsx
+++ b/src/inserted/contrato_insert_sucess.xlsx
@@ -546,7 +546,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>154042</t>
+          <t>154043</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '154042', 'atualiza_campos': [{'tipo': 'i', 'campo': 'data_desistencia', 'valor': ''}, {'tipo': 's', 'campo': 'status', 'valor': 'P'}, {'tipo': 'i', 'campo': 'id_cliente', 'valor': '117693'}, {'tipo': 'i', 'campo': 'data_ativacao', 'valor': ''}, {'tipo': 'd', 'campo': 'data_renovacao', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_avisar_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_bloquear_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cancelamento', 'valor': ''}, {'tipo': 'd', 'campo': 'dt_ult_bloq_manual', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cadastro_sistema', 'valor': '2025-03-19'}]}</t>
+          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '154043', 'atualiza_campos': [{'tipo': 'i', 'campo': 'data_desistencia', 'valor': ''}, {'tipo': 's', 'campo': 'status', 'valor': 'P'}, {'tipo': 'i', 'campo': 'id_cliente', 'valor': '117693'}, {'tipo': 'i', 'campo': 'data_ativacao', 'valor': ''}, {'tipo': 'd', 'campo': 'data_renovacao', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_avisar_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_bloquear_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cancelamento', 'valor': ''}, {'tipo': 'd', 'campo': 'dt_ult_bloq_manual', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cadastro_sistema', 'valor': '2025-03-19'}]}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add database connection settings and new user insertion function
</commit_message>
<xml_diff>
--- a/src/inserted/contrato_insert_sucess.xlsx
+++ b/src/inserted/contrato_insert_sucess.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,15 +481,25 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Senha</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>idContratoIXC</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>statusInsercao</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>logRetorno</t>
         </is>
@@ -546,17 +556,27 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>154044</t>
+          <t>teste1@radios.com</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>peixoto</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>154045</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>sucesso</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '154044', 'atualiza_campos': [{'tipo': 'i', 'campo': 'data_desistencia', 'valor': ''}, {'tipo': 's', 'campo': 'status', 'valor': 'P'}, {'tipo': 'i', 'campo': 'id_cliente', 'valor': '117695'}, {'tipo': 'i', 'campo': 'data_ativacao', 'valor': ''}, {'tipo': 'd', 'campo': 'data_renovacao', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_avisar_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_bloquear_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cancelamento', 'valor': ''}, {'tipo': 'd', 'campo': 'dt_ult_bloq_manual', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cadastro_sistema', 'valor': '2025-03-19'}]}</t>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '154045', 'atualiza_campos': [{'tipo': 'i', 'campo': 'data_desistencia', 'valor': ''}, {'tipo': 's', 'campo': 'status', 'valor': 'P'}, {'tipo': 'i', 'campo': 'id_cliente', 'valor': '117695'}, {'tipo': 'i', 'campo': 'data_ativacao', 'valor': ''}, {'tipo': 'd', 'campo': 'data_renovacao', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_avisar_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'nao_bloquear_ate', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cancelamento', 'valor': ''}, {'tipo': 'd', 'campo': 'dt_ult_bloq_manual', 'valor': ''}, {'tipo': 'd', 'campo': 'data_cadastro_sistema', 'valor': '2025-03-19'}]}</t>
         </is>
       </c>
     </row>

</xml_diff>